<commit_message>
Fixed issues with the data and moved metadata files
</commit_message>
<xml_diff>
--- a/SpaceX CRS-13/Excel/analysed.xlsx
+++ b/SpaceX CRS-13/Excel/analysed.xlsx
@@ -128,12 +128,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$A$2:$A$535</f>
+              <f>Sheet!$A$2:$A$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$B$2:$B$535</f>
+              <f>Sheet!$B$2:$B$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -160,12 +160,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$A$2:$A$535</f>
+              <f>Sheet!$A$2:$A$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$D$2:$D$535</f>
+              <f>Sheet!$D$2:$D$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -192,12 +192,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$A$2:$A$535</f>
+              <f>Sheet!$A$2:$A$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$E$2:$E$535</f>
+              <f>Sheet!$E$2:$E$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -296,12 +296,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$A$2:$A$535</f>
+              <f>Sheet!$A$2:$A$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$C$2:$C$535</f>
+              <f>Sheet!$C$2:$C$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -400,12 +400,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$A$2:$A$535</f>
+              <f>Sheet!$A$2:$A$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$G$2:$G$535</f>
+              <f>Sheet!$G$2:$G$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -504,12 +504,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$A$2:$A$535</f>
+              <f>Sheet!$A$2:$A$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$F$2:$F$535</f>
+              <f>Sheet!$F$2:$F$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -608,12 +608,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$A$2:$A$535</f>
+              <f>Sheet!$A$2:$A$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$H$2:$H$535</f>
+              <f>Sheet!$H$2:$H$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -712,12 +712,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$B$2:$B$535</f>
+              <f>Sheet!$B$2:$B$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$C$2:$C$535</f>
+              <f>Sheet!$C$2:$C$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -816,12 +816,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$F$2:$F$535</f>
+              <f>Sheet!$F$2:$F$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$C$2:$C$535</f>
+              <f>Sheet!$C$2:$C$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -920,12 +920,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$H$2:$H$535</f>
+              <f>Sheet!$H$2:$H$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$C$2:$C$535</f>
+              <f>Sheet!$C$2:$C$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -1024,12 +1024,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>Sheet!$G$2:$G$535</f>
+              <f>Sheet!$G$2:$G$420</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>Sheet!$C$2:$C$535</f>
+              <f>Sheet!$C$2:$C$420</f>
             </numRef>
           </yVal>
         </ser>
@@ -1579,7 +1579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I535"/>
+  <dimension ref="A1:I420"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13767,3341 +13767,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:9">
-      <c r="A421" t="n">
-        <v>419</v>
-      </c>
-      <c r="B421" t="n">
-        <v>4011.328</v>
-      </c>
-      <c r="C421" t="n">
-        <v>215.499</v>
-      </c>
-      <c r="D421" t="n">
-        <v>9.978</v>
-      </c>
-      <c r="E421" t="n">
-        <v>4011.328</v>
-      </c>
-      <c r="F421" t="n">
-        <v>20.929</v>
-      </c>
-      <c r="G421" t="n">
-        <v>669.533</v>
-      </c>
-      <c r="H421" t="n">
-        <v>0.295</v>
-      </c>
-      <c r="I421" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="422" spans="1:9">
-      <c r="A422" t="n">
-        <v>420</v>
-      </c>
-      <c r="B422" t="n">
-        <v>4035.417</v>
-      </c>
-      <c r="C422" t="n">
-        <v>215.496</v>
-      </c>
-      <c r="D422" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="E422" t="n">
-        <v>4035.417</v>
-      </c>
-      <c r="F422" t="n">
-        <v>22.578</v>
-      </c>
-      <c r="G422" t="n">
-        <v>673.556</v>
-      </c>
-      <c r="H422" t="n">
-        <v>0.182</v>
-      </c>
-      <c r="I422" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="423" spans="1:9">
-      <c r="A423" t="n">
-        <v>421</v>
-      </c>
-      <c r="B423" t="n">
-        <v>4059.506</v>
-      </c>
-      <c r="C423" t="n">
-        <v>215.491</v>
-      </c>
-      <c r="D423" t="n">
-        <v>-3.077</v>
-      </c>
-      <c r="E423" t="n">
-        <v>4059.476</v>
-      </c>
-      <c r="F423" t="n">
-        <v>23.963</v>
-      </c>
-      <c r="G423" t="n">
-        <v>677.604</v>
-      </c>
-      <c r="H423" t="n">
-        <v>0.08400000000000001</v>
-      </c>
-      <c r="I423" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="424" spans="1:9">
-      <c r="A424" t="n">
-        <v>422</v>
-      </c>
-      <c r="B424" t="n">
-        <v>4083.595</v>
-      </c>
-      <c r="C424" t="n">
-        <v>215.484</v>
-      </c>
-      <c r="D424" t="n">
-        <v>-6.016</v>
-      </c>
-      <c r="E424" t="n">
-        <v>4082.874</v>
-      </c>
-      <c r="F424" t="n">
-        <v>24.09</v>
-      </c>
-      <c r="G424" t="n">
-        <v>681.675</v>
-      </c>
-      <c r="H424" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="I424" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="425" spans="1:9">
-      <c r="A425" t="n">
-        <v>423</v>
-      </c>
-      <c r="B425" t="n">
-        <v>4107.683</v>
-      </c>
-      <c r="C425" t="n">
-        <v>215.476</v>
-      </c>
-      <c r="D425" t="n">
-        <v>-7.965</v>
-      </c>
-      <c r="E425" t="n">
-        <v>4106.795</v>
-      </c>
-      <c r="F425" t="n">
-        <v>24.08</v>
-      </c>
-      <c r="G425" t="n">
-        <v>685.77</v>
-      </c>
-      <c r="H425" t="n">
-        <v>-0.059</v>
-      </c>
-      <c r="I425" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="426" spans="1:9">
-      <c r="A426" t="n">
-        <v>424</v>
-      </c>
-      <c r="B426" t="n">
-        <v>4131.772</v>
-      </c>
-      <c r="C426" t="n">
-        <v>215.467</v>
-      </c>
-      <c r="D426" t="n">
-        <v>-9.481</v>
-      </c>
-      <c r="E426" t="n">
-        <v>4131.076</v>
-      </c>
-      <c r="F426" t="n">
-        <v>24.072</v>
-      </c>
-      <c r="G426" t="n">
-        <v>689.889</v>
-      </c>
-      <c r="H426" t="n">
-        <v>-0.106</v>
-      </c>
-      <c r="I426" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="427" spans="1:9">
-      <c r="A427" t="n">
-        <v>425</v>
-      </c>
-      <c r="B427" t="n">
-        <v>4155.861</v>
-      </c>
-      <c r="C427" t="n">
-        <v>215.456</v>
-      </c>
-      <c r="D427" t="n">
-        <v>-10.945</v>
-      </c>
-      <c r="E427" t="n">
-        <v>4155.49</v>
-      </c>
-      <c r="F427" t="n">
-        <v>24.067</v>
-      </c>
-      <c r="G427" t="n">
-        <v>694.032</v>
-      </c>
-      <c r="H427" t="n">
-        <v>-0.141</v>
-      </c>
-      <c r="I427" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="428" spans="1:9">
-      <c r="A428" t="n">
-        <v>426</v>
-      </c>
-      <c r="B428" t="n">
-        <v>4179.95</v>
-      </c>
-      <c r="C428" t="n">
-        <v>215.443</v>
-      </c>
-      <c r="D428" t="n">
-        <v>-12.409</v>
-      </c>
-      <c r="E428" t="n">
-        <v>4179.826</v>
-      </c>
-      <c r="F428" t="n">
-        <v>24.062</v>
-      </c>
-      <c r="G428" t="n">
-        <v>698.199</v>
-      </c>
-      <c r="H428" t="n">
-        <v>-0.167</v>
-      </c>
-      <c r="I428" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="429" spans="1:9">
-      <c r="A429" t="n">
-        <v>427</v>
-      </c>
-      <c r="B429" t="n">
-        <v>4204.039</v>
-      </c>
-      <c r="C429" t="n">
-        <v>215.43</v>
-      </c>
-      <c r="D429" t="n">
-        <v>-13.874</v>
-      </c>
-      <c r="E429" t="n">
-        <v>4204.016</v>
-      </c>
-      <c r="F429" t="n">
-        <v>24.059</v>
-      </c>
-      <c r="G429" t="n">
-        <v>702.391</v>
-      </c>
-      <c r="H429" t="n">
-        <v>-0.188</v>
-      </c>
-      <c r="I429" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="430" spans="1:9">
-      <c r="A430" t="n">
-        <v>428</v>
-      </c>
-      <c r="B430" t="n">
-        <v>4228.128</v>
-      </c>
-      <c r="C430" t="n">
-        <v>215.414</v>
-      </c>
-      <c r="D430" t="n">
-        <v>-15.34</v>
-      </c>
-      <c r="E430" t="n">
-        <v>4228.099</v>
-      </c>
-      <c r="F430" t="n">
-        <v>24.056</v>
-      </c>
-      <c r="G430" t="n">
-        <v>706.607</v>
-      </c>
-      <c r="H430" t="n">
-        <v>-0.207</v>
-      </c>
-      <c r="I430" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="431" spans="1:9">
-      <c r="A431" t="n">
-        <v>429</v>
-      </c>
-      <c r="B431" t="n">
-        <v>4252.216</v>
-      </c>
-      <c r="C431" t="n">
-        <v>215.397</v>
-      </c>
-      <c r="D431" t="n">
-        <v>-16.806</v>
-      </c>
-      <c r="E431" t="n">
-        <v>4252.183</v>
-      </c>
-      <c r="F431" t="n">
-        <v>24.053</v>
-      </c>
-      <c r="G431" t="n">
-        <v>710.848</v>
-      </c>
-      <c r="H431" t="n">
-        <v>-0.225</v>
-      </c>
-      <c r="I431" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="432" spans="1:9">
-      <c r="A432" t="n">
-        <v>430</v>
-      </c>
-      <c r="B432" t="n">
-        <v>4276.305</v>
-      </c>
-      <c r="C432" t="n">
-        <v>215.379</v>
-      </c>
-      <c r="D432" t="n">
-        <v>-18.272</v>
-      </c>
-      <c r="E432" t="n">
-        <v>4276.266</v>
-      </c>
-      <c r="F432" t="n">
-        <v>24.05</v>
-      </c>
-      <c r="G432" t="n">
-        <v>715.112</v>
-      </c>
-      <c r="H432" t="n">
-        <v>-0.244</v>
-      </c>
-      <c r="I432" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="433" spans="1:9">
-      <c r="A433" t="n">
-        <v>431</v>
-      </c>
-      <c r="B433" t="n">
-        <v>4300.394</v>
-      </c>
-      <c r="C433" t="n">
-        <v>215.359</v>
-      </c>
-      <c r="D433" t="n">
-        <v>-19.739</v>
-      </c>
-      <c r="E433" t="n">
-        <v>4300.349</v>
-      </c>
-      <c r="F433" t="n">
-        <v>24.047</v>
-      </c>
-      <c r="G433" t="n">
-        <v>719.4</v>
-      </c>
-      <c r="H433" t="n">
-        <v>-0.262</v>
-      </c>
-      <c r="I433" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="434" spans="1:9">
-      <c r="A434" t="n">
-        <v>432</v>
-      </c>
-      <c r="B434" t="n">
-        <v>4324.483</v>
-      </c>
-      <c r="C434" t="n">
-        <v>215.338</v>
-      </c>
-      <c r="D434" t="n">
-        <v>-21.207</v>
-      </c>
-      <c r="E434" t="n">
-        <v>4324.431</v>
-      </c>
-      <c r="F434" t="n">
-        <v>24.044</v>
-      </c>
-      <c r="G434" t="n">
-        <v>723.713</v>
-      </c>
-      <c r="H434" t="n">
-        <v>-0.28</v>
-      </c>
-      <c r="I434" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="435" spans="1:9">
-      <c r="A435" t="n">
-        <v>433</v>
-      </c>
-      <c r="B435" t="n">
-        <v>4348.572</v>
-      </c>
-      <c r="C435" t="n">
-        <v>215.315</v>
-      </c>
-      <c r="D435" t="n">
-        <v>-22.675</v>
-      </c>
-      <c r="E435" t="n">
-        <v>4348.512</v>
-      </c>
-      <c r="F435" t="n">
-        <v>24.041</v>
-      </c>
-      <c r="G435" t="n">
-        <v>728.049</v>
-      </c>
-      <c r="H435" t="n">
-        <v>-0.298</v>
-      </c>
-      <c r="I435" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="436" spans="1:9">
-      <c r="A436" t="n">
-        <v>434</v>
-      </c>
-      <c r="B436" t="n">
-        <v>4372.66</v>
-      </c>
-      <c r="C436" t="n">
-        <v>215.291</v>
-      </c>
-      <c r="D436" t="n">
-        <v>-24.143</v>
-      </c>
-      <c r="E436" t="n">
-        <v>4372.594</v>
-      </c>
-      <c r="F436" t="n">
-        <v>24.038</v>
-      </c>
-      <c r="G436" t="n">
-        <v>732.41</v>
-      </c>
-      <c r="H436" t="n">
-        <v>-0.315</v>
-      </c>
-      <c r="I436" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="437" spans="1:9">
-      <c r="A437" t="n">
-        <v>435</v>
-      </c>
-      <c r="B437" t="n">
-        <v>4396.749</v>
-      </c>
-      <c r="C437" t="n">
-        <v>215.266</v>
-      </c>
-      <c r="D437" t="n">
-        <v>-25.612</v>
-      </c>
-      <c r="E437" t="n">
-        <v>4396.674</v>
-      </c>
-      <c r="F437" t="n">
-        <v>24.035</v>
-      </c>
-      <c r="G437" t="n">
-        <v>736.794</v>
-      </c>
-      <c r="H437" t="n">
-        <v>-0.333</v>
-      </c>
-      <c r="I437" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="438" spans="1:9">
-      <c r="A438" t="n">
-        <v>436</v>
-      </c>
-      <c r="B438" t="n">
-        <v>4420.838</v>
-      </c>
-      <c r="C438" t="n">
-        <v>215.239</v>
-      </c>
-      <c r="D438" t="n">
-        <v>-27.082</v>
-      </c>
-      <c r="E438" t="n">
-        <v>4420.755</v>
-      </c>
-      <c r="F438" t="n">
-        <v>24.033</v>
-      </c>
-      <c r="G438" t="n">
-        <v>741.203</v>
-      </c>
-      <c r="H438" t="n">
-        <v>-0.35</v>
-      </c>
-      <c r="I438" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="439" spans="1:9">
-      <c r="A439" t="n">
-        <v>437</v>
-      </c>
-      <c r="B439" t="n">
-        <v>4444.927</v>
-      </c>
-      <c r="C439" t="n">
-        <v>215.21</v>
-      </c>
-      <c r="D439" t="n">
-        <v>-28.552</v>
-      </c>
-      <c r="E439" t="n">
-        <v>4444.835</v>
-      </c>
-      <c r="F439" t="n">
-        <v>24.03</v>
-      </c>
-      <c r="G439" t="n">
-        <v>745.636</v>
-      </c>
-      <c r="H439" t="n">
-        <v>-0.367</v>
-      </c>
-      <c r="I439" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="440" spans="1:9">
-      <c r="A440" t="n">
-        <v>438</v>
-      </c>
-      <c r="B440" t="n">
-        <v>4469.016</v>
-      </c>
-      <c r="C440" t="n">
-        <v>215.18</v>
-      </c>
-      <c r="D440" t="n">
-        <v>-30.022</v>
-      </c>
-      <c r="E440" t="n">
-        <v>4468.915</v>
-      </c>
-      <c r="F440" t="n">
-        <v>24.027</v>
-      </c>
-      <c r="G440" t="n">
-        <v>750.093</v>
-      </c>
-      <c r="H440" t="n">
-        <v>-0.384</v>
-      </c>
-      <c r="I440" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="441" spans="1:9">
-      <c r="A441" t="n">
-        <v>439</v>
-      </c>
-      <c r="B441" t="n">
-        <v>4493.104</v>
-      </c>
-      <c r="C441" t="n">
-        <v>215.149</v>
-      </c>
-      <c r="D441" t="n">
-        <v>-31.493</v>
-      </c>
-      <c r="E441" t="n">
-        <v>4492.994</v>
-      </c>
-      <c r="F441" t="n">
-        <v>24.024</v>
-      </c>
-      <c r="G441" t="n">
-        <v>754.574</v>
-      </c>
-      <c r="H441" t="n">
-        <v>-0.401</v>
-      </c>
-      <c r="I441" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="442" spans="1:9">
-      <c r="A442" t="n">
-        <v>440</v>
-      </c>
-      <c r="B442" t="n">
-        <v>4517.193</v>
-      </c>
-      <c r="C442" t="n">
-        <v>215.116</v>
-      </c>
-      <c r="D442" t="n">
-        <v>-32.965</v>
-      </c>
-      <c r="E442" t="n">
-        <v>4517.073</v>
-      </c>
-      <c r="F442" t="n">
-        <v>24.022</v>
-      </c>
-      <c r="G442" t="n">
-        <v>759.079</v>
-      </c>
-      <c r="H442" t="n">
-        <v>-0.417</v>
-      </c>
-      <c r="I442" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="443" spans="1:9">
-      <c r="A443" t="n">
-        <v>441</v>
-      </c>
-      <c r="B443" t="n">
-        <v>4541.282</v>
-      </c>
-      <c r="C443" t="n">
-        <v>215.081</v>
-      </c>
-      <c r="D443" t="n">
-        <v>-34.437</v>
-      </c>
-      <c r="E443" t="n">
-        <v>4541.151</v>
-      </c>
-      <c r="F443" t="n">
-        <v>24.019</v>
-      </c>
-      <c r="G443" t="n">
-        <v>763.6079999999999</v>
-      </c>
-      <c r="H443" t="n">
-        <v>-0.433</v>
-      </c>
-      <c r="I443" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="444" spans="1:9">
-      <c r="A444" t="n">
-        <v>442</v>
-      </c>
-      <c r="B444" t="n">
-        <v>4565.371</v>
-      </c>
-      <c r="C444" t="n">
-        <v>215.045</v>
-      </c>
-      <c r="D444" t="n">
-        <v>-35.909</v>
-      </c>
-      <c r="E444" t="n">
-        <v>4565.23</v>
-      </c>
-      <c r="F444" t="n">
-        <v>24.017</v>
-      </c>
-      <c r="G444" t="n">
-        <v>768.1609999999999</v>
-      </c>
-      <c r="H444" t="n">
-        <v>-0.45</v>
-      </c>
-      <c r="I444" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="445" spans="1:9">
-      <c r="A445" t="n">
-        <v>443</v>
-      </c>
-      <c r="B445" t="n">
-        <v>4589.46</v>
-      </c>
-      <c r="C445" t="n">
-        <v>215.008</v>
-      </c>
-      <c r="D445" t="n">
-        <v>-37.382</v>
-      </c>
-      <c r="E445" t="n">
-        <v>4589.307</v>
-      </c>
-      <c r="F445" t="n">
-        <v>24.014</v>
-      </c>
-      <c r="G445" t="n">
-        <v>772.7380000000001</v>
-      </c>
-      <c r="H445" t="n">
-        <v>-0.466</v>
-      </c>
-      <c r="I445" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="446" spans="1:9">
-      <c r="A446" t="n">
-        <v>444</v>
-      </c>
-      <c r="B446" t="n">
-        <v>4613.549</v>
-      </c>
-      <c r="C446" t="n">
-        <v>214.969</v>
-      </c>
-      <c r="D446" t="n">
-        <v>-38.856</v>
-      </c>
-      <c r="E446" t="n">
-        <v>4613.385</v>
-      </c>
-      <c r="F446" t="n">
-        <v>24.011</v>
-      </c>
-      <c r="G446" t="n">
-        <v>777.3390000000001</v>
-      </c>
-      <c r="H446" t="n">
-        <v>-0.482</v>
-      </c>
-      <c r="I446" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="447" spans="1:9">
-      <c r="A447" t="n">
-        <v>445</v>
-      </c>
-      <c r="B447" t="n">
-        <v>4637.637</v>
-      </c>
-      <c r="C447" t="n">
-        <v>214.929</v>
-      </c>
-      <c r="D447" t="n">
-        <v>-40.329</v>
-      </c>
-      <c r="E447" t="n">
-        <v>4637.462</v>
-      </c>
-      <c r="F447" t="n">
-        <v>24.009</v>
-      </c>
-      <c r="G447" t="n">
-        <v>781.965</v>
-      </c>
-      <c r="H447" t="n">
-        <v>-0.497</v>
-      </c>
-      <c r="I447" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="448" spans="1:9">
-      <c r="A448" t="n">
-        <v>446</v>
-      </c>
-      <c r="B448" t="n">
-        <v>4661.726</v>
-      </c>
-      <c r="C448" t="n">
-        <v>214.887</v>
-      </c>
-      <c r="D448" t="n">
-        <v>-41.804</v>
-      </c>
-      <c r="E448" t="n">
-        <v>4661.539</v>
-      </c>
-      <c r="F448" t="n">
-        <v>24.006</v>
-      </c>
-      <c r="G448" t="n">
-        <v>786.614</v>
-      </c>
-      <c r="H448" t="n">
-        <v>-0.513</v>
-      </c>
-      <c r="I448" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="449" spans="1:9">
-      <c r="A449" t="n">
-        <v>447</v>
-      </c>
-      <c r="B449" t="n">
-        <v>4685.815</v>
-      </c>
-      <c r="C449" t="n">
-        <v>214.844</v>
-      </c>
-      <c r="D449" t="n">
-        <v>-43.279</v>
-      </c>
-      <c r="E449" t="n">
-        <v>4685.615</v>
-      </c>
-      <c r="F449" t="n">
-        <v>24.004</v>
-      </c>
-      <c r="G449" t="n">
-        <v>791.288</v>
-      </c>
-      <c r="H449" t="n">
-        <v>-0.528</v>
-      </c>
-      <c r="I449" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="450" spans="1:9">
-      <c r="A450" t="n">
-        <v>448</v>
-      </c>
-      <c r="B450" t="n">
-        <v>4709.904</v>
-      </c>
-      <c r="C450" t="n">
-        <v>214.799</v>
-      </c>
-      <c r="D450" t="n">
-        <v>-44.754</v>
-      </c>
-      <c r="E450" t="n">
-        <v>4709.691</v>
-      </c>
-      <c r="F450" t="n">
-        <v>24.001</v>
-      </c>
-      <c r="G450" t="n">
-        <v>795.986</v>
-      </c>
-      <c r="H450" t="n">
-        <v>-0.544</v>
-      </c>
-      <c r="I450" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="451" spans="1:9">
-      <c r="A451" t="n">
-        <v>449</v>
-      </c>
-      <c r="B451" t="n">
-        <v>4733.993</v>
-      </c>
-      <c r="C451" t="n">
-        <v>214.753</v>
-      </c>
-      <c r="D451" t="n">
-        <v>-46.23</v>
-      </c>
-      <c r="E451" t="n">
-        <v>4733.767</v>
-      </c>
-      <c r="F451" t="n">
-        <v>23.999</v>
-      </c>
-      <c r="G451" t="n">
-        <v>800.707</v>
-      </c>
-      <c r="H451" t="n">
-        <v>-0.5590000000000001</v>
-      </c>
-      <c r="I451" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="452" spans="1:9">
-      <c r="A452" t="n">
-        <v>450</v>
-      </c>
-      <c r="B452" t="n">
-        <v>4758.081</v>
-      </c>
-      <c r="C452" t="n">
-        <v>214.705</v>
-      </c>
-      <c r="D452" t="n">
-        <v>-47.707</v>
-      </c>
-      <c r="E452" t="n">
-        <v>4757.842</v>
-      </c>
-      <c r="F452" t="n">
-        <v>23.997</v>
-      </c>
-      <c r="G452" t="n">
-        <v>805.453</v>
-      </c>
-      <c r="H452" t="n">
-        <v>-0.574</v>
-      </c>
-      <c r="I452" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="453" spans="1:9">
-      <c r="A453" t="n">
-        <v>451</v>
-      </c>
-      <c r="B453" t="n">
-        <v>4782.17</v>
-      </c>
-      <c r="C453" t="n">
-        <v>214.656</v>
-      </c>
-      <c r="D453" t="n">
-        <v>-49.183</v>
-      </c>
-      <c r="E453" t="n">
-        <v>4781.917</v>
-      </c>
-      <c r="F453" t="n">
-        <v>23.994</v>
-      </c>
-      <c r="G453" t="n">
-        <v>810.223</v>
-      </c>
-      <c r="H453" t="n">
-        <v>-0.588</v>
-      </c>
-      <c r="I453" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="454" spans="1:9">
-      <c r="A454" t="n">
-        <v>452</v>
-      </c>
-      <c r="B454" t="n">
-        <v>4806.259</v>
-      </c>
-      <c r="C454" t="n">
-        <v>214.605</v>
-      </c>
-      <c r="D454" t="n">
-        <v>-50.661</v>
-      </c>
-      <c r="E454" t="n">
-        <v>4805.992</v>
-      </c>
-      <c r="F454" t="n">
-        <v>23.992</v>
-      </c>
-      <c r="G454" t="n">
-        <v>815.0170000000001</v>
-      </c>
-      <c r="H454" t="n">
-        <v>-0.603</v>
-      </c>
-      <c r="I454" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="455" spans="1:9">
-      <c r="A455" t="n">
-        <v>453</v>
-      </c>
-      <c r="B455" t="n">
-        <v>4830.348</v>
-      </c>
-      <c r="C455" t="n">
-        <v>214.553</v>
-      </c>
-      <c r="D455" t="n">
-        <v>-52.139</v>
-      </c>
-      <c r="E455" t="n">
-        <v>4830.066</v>
-      </c>
-      <c r="F455" t="n">
-        <v>23.99</v>
-      </c>
-      <c r="G455" t="n">
-        <v>819.835</v>
-      </c>
-      <c r="H455" t="n">
-        <v>-0.618</v>
-      </c>
-      <c r="I455" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="456" spans="1:9">
-      <c r="A456" t="n">
-        <v>454</v>
-      </c>
-      <c r="B456" t="n">
-        <v>4854.437</v>
-      </c>
-      <c r="C456" t="n">
-        <v>214.499</v>
-      </c>
-      <c r="D456" t="n">
-        <v>-53.617</v>
-      </c>
-      <c r="E456" t="n">
-        <v>4854.141</v>
-      </c>
-      <c r="F456" t="n">
-        <v>23.987</v>
-      </c>
-      <c r="G456" t="n">
-        <v>824.677</v>
-      </c>
-      <c r="H456" t="n">
-        <v>-0.632</v>
-      </c>
-      <c r="I456" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="457" spans="1:9">
-      <c r="A457" t="n">
-        <v>455</v>
-      </c>
-      <c r="B457" t="n">
-        <v>4878.526</v>
-      </c>
-      <c r="C457" t="n">
-        <v>214.444</v>
-      </c>
-      <c r="D457" t="n">
-        <v>-55.096</v>
-      </c>
-      <c r="E457" t="n">
-        <v>4878.214</v>
-      </c>
-      <c r="F457" t="n">
-        <v>23.985</v>
-      </c>
-      <c r="G457" t="n">
-        <v>829.543</v>
-      </c>
-      <c r="H457" t="n">
-        <v>-0.646</v>
-      </c>
-      <c r="I457" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="458" spans="1:9">
-      <c r="A458" t="n">
-        <v>456</v>
-      </c>
-      <c r="B458" t="n">
-        <v>4902.614</v>
-      </c>
-      <c r="C458" t="n">
-        <v>214.388</v>
-      </c>
-      <c r="D458" t="n">
-        <v>-56.575</v>
-      </c>
-      <c r="E458" t="n">
-        <v>4902.288</v>
-      </c>
-      <c r="F458" t="n">
-        <v>23.983</v>
-      </c>
-      <c r="G458" t="n">
-        <v>834.434</v>
-      </c>
-      <c r="H458" t="n">
-        <v>-0.66</v>
-      </c>
-      <c r="I458" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="459" spans="1:9">
-      <c r="A459" t="n">
-        <v>457</v>
-      </c>
-      <c r="B459" t="n">
-        <v>4926.703</v>
-      </c>
-      <c r="C459" t="n">
-        <v>214.33</v>
-      </c>
-      <c r="D459" t="n">
-        <v>-58.055</v>
-      </c>
-      <c r="E459" t="n">
-        <v>4926.361</v>
-      </c>
-      <c r="F459" t="n">
-        <v>23.98</v>
-      </c>
-      <c r="G459" t="n">
-        <v>839.348</v>
-      </c>
-      <c r="H459" t="n">
-        <v>-0.674</v>
-      </c>
-      <c r="I459" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="460" spans="1:9">
-      <c r="A460" t="n">
-        <v>458</v>
-      </c>
-      <c r="B460" t="n">
-        <v>4950.792</v>
-      </c>
-      <c r="C460" t="n">
-        <v>214.27</v>
-      </c>
-      <c r="D460" t="n">
-        <v>-59.536</v>
-      </c>
-      <c r="E460" t="n">
-        <v>4950.434</v>
-      </c>
-      <c r="F460" t="n">
-        <v>23.978</v>
-      </c>
-      <c r="G460" t="n">
-        <v>844.2859999999999</v>
-      </c>
-      <c r="H460" t="n">
-        <v>-0.6879999999999999</v>
-      </c>
-      <c r="I460" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="461" spans="1:9">
-      <c r="A461" t="n">
-        <v>459</v>
-      </c>
-      <c r="B461" t="n">
-        <v>4974.881</v>
-      </c>
-      <c r="C461" t="n">
-        <v>214.209</v>
-      </c>
-      <c r="D461" t="n">
-        <v>-61.016</v>
-      </c>
-      <c r="E461" t="n">
-        <v>4974.507</v>
-      </c>
-      <c r="F461" t="n">
-        <v>23.976</v>
-      </c>
-      <c r="G461" t="n">
-        <v>849.249</v>
-      </c>
-      <c r="H461" t="n">
-        <v>-0.702</v>
-      </c>
-      <c r="I461" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="462" spans="1:9">
-      <c r="A462" t="n">
-        <v>460</v>
-      </c>
-      <c r="B462" t="n">
-        <v>4998.97</v>
-      </c>
-      <c r="C462" t="n">
-        <v>214.147</v>
-      </c>
-      <c r="D462" t="n">
-        <v>-62.498</v>
-      </c>
-      <c r="E462" t="n">
-        <v>4998.579</v>
-      </c>
-      <c r="F462" t="n">
-        <v>23.974</v>
-      </c>
-      <c r="G462" t="n">
-        <v>854.235</v>
-      </c>
-      <c r="H462" t="n">
-        <v>-0.716</v>
-      </c>
-      <c r="I462" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="463" spans="1:9">
-      <c r="A463" t="n">
-        <v>461</v>
-      </c>
-      <c r="B463" t="n">
-        <v>5023.058</v>
-      </c>
-      <c r="C463" t="n">
-        <v>214.083</v>
-      </c>
-      <c r="D463" t="n">
-        <v>-63.98</v>
-      </c>
-      <c r="E463" t="n">
-        <v>5022.651</v>
-      </c>
-      <c r="F463" t="n">
-        <v>23.972</v>
-      </c>
-      <c r="G463" t="n">
-        <v>859.246</v>
-      </c>
-      <c r="H463" t="n">
-        <v>-0.729</v>
-      </c>
-      <c r="I463" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="464" spans="1:9">
-      <c r="A464" t="n">
-        <v>462</v>
-      </c>
-      <c r="B464" t="n">
-        <v>5047.147</v>
-      </c>
-      <c r="C464" t="n">
-        <v>214.017</v>
-      </c>
-      <c r="D464" t="n">
-        <v>-65.462</v>
-      </c>
-      <c r="E464" t="n">
-        <v>5046.723</v>
-      </c>
-      <c r="F464" t="n">
-        <v>23.969</v>
-      </c>
-      <c r="G464" t="n">
-        <v>864.2809999999999</v>
-      </c>
-      <c r="H464" t="n">
-        <v>-0.742</v>
-      </c>
-      <c r="I464" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="465" spans="1:9">
-      <c r="A465" t="n">
-        <v>463</v>
-      </c>
-      <c r="B465" t="n">
-        <v>5071.236</v>
-      </c>
-      <c r="C465" t="n">
-        <v>213.95</v>
-      </c>
-      <c r="D465" t="n">
-        <v>-66.94499999999999</v>
-      </c>
-      <c r="E465" t="n">
-        <v>5070.794</v>
-      </c>
-      <c r="F465" t="n">
-        <v>23.967</v>
-      </c>
-      <c r="G465" t="n">
-        <v>869.3390000000001</v>
-      </c>
-      <c r="H465" t="n">
-        <v>-0.756</v>
-      </c>
-      <c r="I465" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="466" spans="1:9">
-      <c r="A466" t="n">
-        <v>464</v>
-      </c>
-      <c r="B466" t="n">
-        <v>5095.325</v>
-      </c>
-      <c r="C466" t="n">
-        <v>213.882</v>
-      </c>
-      <c r="D466" t="n">
-        <v>-68.428</v>
-      </c>
-      <c r="E466" t="n">
-        <v>5094.865</v>
-      </c>
-      <c r="F466" t="n">
-        <v>23.965</v>
-      </c>
-      <c r="G466" t="n">
-        <v>874.422</v>
-      </c>
-      <c r="H466" t="n">
-        <v>-0.769</v>
-      </c>
-      <c r="I466" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="467" spans="1:9">
-      <c r="A467" t="n">
-        <v>465</v>
-      </c>
-      <c r="B467" t="n">
-        <v>5119.414</v>
-      </c>
-      <c r="C467" t="n">
-        <v>213.812</v>
-      </c>
-      <c r="D467" t="n">
-        <v>-69.91200000000001</v>
-      </c>
-      <c r="E467" t="n">
-        <v>5118.936</v>
-      </c>
-      <c r="F467" t="n">
-        <v>23.963</v>
-      </c>
-      <c r="G467" t="n">
-        <v>879.529</v>
-      </c>
-      <c r="H467" t="n">
-        <v>-0.782</v>
-      </c>
-      <c r="I467" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="468" spans="1:9">
-      <c r="A468" t="n">
-        <v>466</v>
-      </c>
-      <c r="B468" t="n">
-        <v>5143.503</v>
-      </c>
-      <c r="C468" t="n">
-        <v>213.74</v>
-      </c>
-      <c r="D468" t="n">
-        <v>-71.396</v>
-      </c>
-      <c r="E468" t="n">
-        <v>5143.007</v>
-      </c>
-      <c r="F468" t="n">
-        <v>23.961</v>
-      </c>
-      <c r="G468" t="n">
-        <v>884.66</v>
-      </c>
-      <c r="H468" t="n">
-        <v>-0.795</v>
-      </c>
-      <c r="I468" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="469" spans="1:9">
-      <c r="A469" t="n">
-        <v>467</v>
-      </c>
-      <c r="B469" t="n">
-        <v>5167.591</v>
-      </c>
-      <c r="C469" t="n">
-        <v>213.668</v>
-      </c>
-      <c r="D469" t="n">
-        <v>-72.881</v>
-      </c>
-      <c r="E469" t="n">
-        <v>5167.077</v>
-      </c>
-      <c r="F469" t="n">
-        <v>23.959</v>
-      </c>
-      <c r="G469" t="n">
-        <v>889.8150000000001</v>
-      </c>
-      <c r="H469" t="n">
-        <v>-0.8070000000000001</v>
-      </c>
-      <c r="I469" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="470" spans="1:9">
-      <c r="A470" t="n">
-        <v>468</v>
-      </c>
-      <c r="B470" t="n">
-        <v>5191.68</v>
-      </c>
-      <c r="C470" t="n">
-        <v>213.593</v>
-      </c>
-      <c r="D470" t="n">
-        <v>-74.367</v>
-      </c>
-      <c r="E470" t="n">
-        <v>5191.147</v>
-      </c>
-      <c r="F470" t="n">
-        <v>23.957</v>
-      </c>
-      <c r="G470" t="n">
-        <v>894.994</v>
-      </c>
-      <c r="H470" t="n">
-        <v>-0.82</v>
-      </c>
-      <c r="I470" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="471" spans="1:9">
-      <c r="A471" t="n">
-        <v>469</v>
-      </c>
-      <c r="B471" t="n">
-        <v>5215.769</v>
-      </c>
-      <c r="C471" t="n">
-        <v>213.517</v>
-      </c>
-      <c r="D471" t="n">
-        <v>-75.852</v>
-      </c>
-      <c r="E471" t="n">
-        <v>5215.217</v>
-      </c>
-      <c r="F471" t="n">
-        <v>23.955</v>
-      </c>
-      <c r="G471" t="n">
-        <v>900.197</v>
-      </c>
-      <c r="H471" t="n">
-        <v>-0.833</v>
-      </c>
-      <c r="I471" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="472" spans="1:9">
-      <c r="A472" t="n">
-        <v>470</v>
-      </c>
-      <c r="B472" t="n">
-        <v>5239.858</v>
-      </c>
-      <c r="C472" t="n">
-        <v>213.44</v>
-      </c>
-      <c r="D472" t="n">
-        <v>-77.339</v>
-      </c>
-      <c r="E472" t="n">
-        <v>5239.287</v>
-      </c>
-      <c r="F472" t="n">
-        <v>23.953</v>
-      </c>
-      <c r="G472" t="n">
-        <v>905.425</v>
-      </c>
-      <c r="H472" t="n">
-        <v>-0.845</v>
-      </c>
-      <c r="I472" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="473" spans="1:9">
-      <c r="A473" t="n">
-        <v>471</v>
-      </c>
-      <c r="B473" t="n">
-        <v>5263.947</v>
-      </c>
-      <c r="C473" t="n">
-        <v>213.361</v>
-      </c>
-      <c r="D473" t="n">
-        <v>-78.825</v>
-      </c>
-      <c r="E473" t="n">
-        <v>5263.356</v>
-      </c>
-      <c r="F473" t="n">
-        <v>23.951</v>
-      </c>
-      <c r="G473" t="n">
-        <v>910.676</v>
-      </c>
-      <c r="H473" t="n">
-        <v>-0.857</v>
-      </c>
-      <c r="I473" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="474" spans="1:9">
-      <c r="A474" t="n">
-        <v>472</v>
-      </c>
-      <c r="B474" t="n">
-        <v>5288.035</v>
-      </c>
-      <c r="C474" t="n">
-        <v>213.281</v>
-      </c>
-      <c r="D474" t="n">
-        <v>-80.313</v>
-      </c>
-      <c r="E474" t="n">
-        <v>5287.425</v>
-      </c>
-      <c r="F474" t="n">
-        <v>23.949</v>
-      </c>
-      <c r="G474" t="n">
-        <v>915.951</v>
-      </c>
-      <c r="H474" t="n">
-        <v>-0.87</v>
-      </c>
-      <c r="I474" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="475" spans="1:9">
-      <c r="A475" t="n">
-        <v>473</v>
-      </c>
-      <c r="B475" t="n">
-        <v>5312.124</v>
-      </c>
-      <c r="C475" t="n">
-        <v>213.199</v>
-      </c>
-      <c r="D475" t="n">
-        <v>-81.801</v>
-      </c>
-      <c r="E475" t="n">
-        <v>5311.494</v>
-      </c>
-      <c r="F475" t="n">
-        <v>23.947</v>
-      </c>
-      <c r="G475" t="n">
-        <v>921.251</v>
-      </c>
-      <c r="H475" t="n">
-        <v>-0.882</v>
-      </c>
-      <c r="I475" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="476" spans="1:9">
-      <c r="A476" t="n">
-        <v>474</v>
-      </c>
-      <c r="B476" t="n">
-        <v>5336.213</v>
-      </c>
-      <c r="C476" t="n">
-        <v>213.116</v>
-      </c>
-      <c r="D476" t="n">
-        <v>-83.289</v>
-      </c>
-      <c r="E476" t="n">
-        <v>5335.563</v>
-      </c>
-      <c r="F476" t="n">
-        <v>23.945</v>
-      </c>
-      <c r="G476" t="n">
-        <v>926.574</v>
-      </c>
-      <c r="H476" t="n">
-        <v>-0.894</v>
-      </c>
-      <c r="I476" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="477" spans="1:9">
-      <c r="A477" t="n">
-        <v>475</v>
-      </c>
-      <c r="B477" t="n">
-        <v>5360.302</v>
-      </c>
-      <c r="C477" t="n">
-        <v>213.031</v>
-      </c>
-      <c r="D477" t="n">
-        <v>-84.77800000000001</v>
-      </c>
-      <c r="E477" t="n">
-        <v>5359.631</v>
-      </c>
-      <c r="F477" t="n">
-        <v>23.943</v>
-      </c>
-      <c r="G477" t="n">
-        <v>931.922</v>
-      </c>
-      <c r="H477" t="n">
-        <v>-0.906</v>
-      </c>
-      <c r="I477" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="478" spans="1:9">
-      <c r="A478" t="n">
-        <v>476</v>
-      </c>
-      <c r="B478" t="n">
-        <v>5384.391</v>
-      </c>
-      <c r="C478" t="n">
-        <v>212.945</v>
-      </c>
-      <c r="D478" t="n">
-        <v>-86.267</v>
-      </c>
-      <c r="E478" t="n">
-        <v>5383.699</v>
-      </c>
-      <c r="F478" t="n">
-        <v>23.941</v>
-      </c>
-      <c r="G478" t="n">
-        <v>937.294</v>
-      </c>
-      <c r="H478" t="n">
-        <v>-0.917</v>
-      </c>
-      <c r="I478" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="479" spans="1:9">
-      <c r="A479" t="n">
-        <v>477</v>
-      </c>
-      <c r="B479" t="n">
-        <v>5408.48</v>
-      </c>
-      <c r="C479" t="n">
-        <v>212.857</v>
-      </c>
-      <c r="D479" t="n">
-        <v>-87.75700000000001</v>
-      </c>
-      <c r="E479" t="n">
-        <v>5407.767</v>
-      </c>
-      <c r="F479" t="n">
-        <v>23.939</v>
-      </c>
-      <c r="G479" t="n">
-        <v>942.689</v>
-      </c>
-      <c r="H479" t="n">
-        <v>-0.929</v>
-      </c>
-      <c r="I479" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="480" spans="1:9">
-      <c r="A480" t="n">
-        <v>478</v>
-      </c>
-      <c r="B480" t="n">
-        <v>5432.568</v>
-      </c>
-      <c r="C480" t="n">
-        <v>212.768</v>
-      </c>
-      <c r="D480" t="n">
-        <v>-89.247</v>
-      </c>
-      <c r="E480" t="n">
-        <v>5431.835</v>
-      </c>
-      <c r="F480" t="n">
-        <v>23.938</v>
-      </c>
-      <c r="G480" t="n">
-        <v>948.109</v>
-      </c>
-      <c r="H480" t="n">
-        <v>-0.9409999999999999</v>
-      </c>
-      <c r="I480" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="481" spans="1:9">
-      <c r="A481" t="n">
-        <v>479</v>
-      </c>
-      <c r="B481" t="n">
-        <v>5456.657</v>
-      </c>
-      <c r="C481" t="n">
-        <v>212.677</v>
-      </c>
-      <c r="D481" t="n">
-        <v>-90.738</v>
-      </c>
-      <c r="E481" t="n">
-        <v>5455.903</v>
-      </c>
-      <c r="F481" t="n">
-        <v>23.936</v>
-      </c>
-      <c r="G481" t="n">
-        <v>953.553</v>
-      </c>
-      <c r="H481" t="n">
-        <v>-0.952</v>
-      </c>
-      <c r="I481" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="482" spans="1:9">
-      <c r="A482" t="n">
-        <v>480</v>
-      </c>
-      <c r="B482" t="n">
-        <v>5480.746</v>
-      </c>
-      <c r="C482" t="n">
-        <v>212.585</v>
-      </c>
-      <c r="D482" t="n">
-        <v>-92.229</v>
-      </c>
-      <c r="E482" t="n">
-        <v>5479.97</v>
-      </c>
-      <c r="F482" t="n">
-        <v>23.934</v>
-      </c>
-      <c r="G482" t="n">
-        <v>959.021</v>
-      </c>
-      <c r="H482" t="n">
-        <v>-0.964</v>
-      </c>
-      <c r="I482" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="483" spans="1:9">
-      <c r="A483" t="n">
-        <v>481</v>
-      </c>
-      <c r="B483" t="n">
-        <v>5504.835</v>
-      </c>
-      <c r="C483" t="n">
-        <v>212.491</v>
-      </c>
-      <c r="D483" t="n">
-        <v>-93.721</v>
-      </c>
-      <c r="E483" t="n">
-        <v>5504.037</v>
-      </c>
-      <c r="F483" t="n">
-        <v>23.932</v>
-      </c>
-      <c r="G483" t="n">
-        <v>964.513</v>
-      </c>
-      <c r="H483" t="n">
-        <v>-0.975</v>
-      </c>
-      <c r="I483" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="484" spans="1:9">
-      <c r="A484" t="n">
-        <v>482</v>
-      </c>
-      <c r="B484" t="n">
-        <v>5528.924</v>
-      </c>
-      <c r="C484" t="n">
-        <v>212.396</v>
-      </c>
-      <c r="D484" t="n">
-        <v>-95.21299999999999</v>
-      </c>
-      <c r="E484" t="n">
-        <v>5528.104</v>
-      </c>
-      <c r="F484" t="n">
-        <v>23.93</v>
-      </c>
-      <c r="G484" t="n">
-        <v>970.029</v>
-      </c>
-      <c r="H484" t="n">
-        <v>-0.986</v>
-      </c>
-      <c r="I484" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="485" spans="1:9">
-      <c r="A485" t="n">
-        <v>483</v>
-      </c>
-      <c r="B485" t="n">
-        <v>5553.012</v>
-      </c>
-      <c r="C485" t="n">
-        <v>212.299</v>
-      </c>
-      <c r="D485" t="n">
-        <v>-96.706</v>
-      </c>
-      <c r="E485" t="n">
-        <v>5552.17</v>
-      </c>
-      <c r="F485" t="n">
-        <v>23.928</v>
-      </c>
-      <c r="G485" t="n">
-        <v>975.569</v>
-      </c>
-      <c r="H485" t="n">
-        <v>-0.997</v>
-      </c>
-      <c r="I485" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="486" spans="1:9">
-      <c r="A486" t="n">
-        <v>484</v>
-      </c>
-      <c r="B486" t="n">
-        <v>5577.101</v>
-      </c>
-      <c r="C486" t="n">
-        <v>212.201</v>
-      </c>
-      <c r="D486" t="n">
-        <v>-98.199</v>
-      </c>
-      <c r="E486" t="n">
-        <v>5576.237</v>
-      </c>
-      <c r="F486" t="n">
-        <v>23.927</v>
-      </c>
-      <c r="G486" t="n">
-        <v>981.133</v>
-      </c>
-      <c r="H486" t="n">
-        <v>-1.008</v>
-      </c>
-      <c r="I486" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="487" spans="1:9">
-      <c r="A487" t="n">
-        <v>485</v>
-      </c>
-      <c r="B487" t="n">
-        <v>5601.19</v>
-      </c>
-      <c r="C487" t="n">
-        <v>212.101</v>
-      </c>
-      <c r="D487" t="n">
-        <v>-99.693</v>
-      </c>
-      <c r="E487" t="n">
-        <v>5600.303</v>
-      </c>
-      <c r="F487" t="n">
-        <v>23.925</v>
-      </c>
-      <c r="G487" t="n">
-        <v>986.722</v>
-      </c>
-      <c r="H487" t="n">
-        <v>-1.019</v>
-      </c>
-      <c r="I487" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="488" spans="1:9">
-      <c r="A488" t="n">
-        <v>486</v>
-      </c>
-      <c r="B488" t="n">
-        <v>5625.279</v>
-      </c>
-      <c r="C488" t="n">
-        <v>212</v>
-      </c>
-      <c r="D488" t="n">
-        <v>-101.187</v>
-      </c>
-      <c r="E488" t="n">
-        <v>5624.369</v>
-      </c>
-      <c r="F488" t="n">
-        <v>23.923</v>
-      </c>
-      <c r="G488" t="n">
-        <v>992.3339999999999</v>
-      </c>
-      <c r="H488" t="n">
-        <v>-1.03</v>
-      </c>
-      <c r="I488" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="489" spans="1:9">
-      <c r="A489" t="n">
-        <v>487</v>
-      </c>
-      <c r="B489" t="n">
-        <v>5649.368</v>
-      </c>
-      <c r="C489" t="n">
-        <v>211.897</v>
-      </c>
-      <c r="D489" t="n">
-        <v>-102.682</v>
-      </c>
-      <c r="E489" t="n">
-        <v>5648.373</v>
-      </c>
-      <c r="F489" t="n">
-        <v>23.921</v>
-      </c>
-      <c r="G489" t="n">
-        <v>997.97</v>
-      </c>
-      <c r="H489" t="n">
-        <v>-1.041</v>
-      </c>
-      <c r="I489" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="490" spans="1:9">
-      <c r="A490" t="n">
-        <v>488</v>
-      </c>
-      <c r="B490" t="n">
-        <v>5673.456</v>
-      </c>
-      <c r="C490" t="n">
-        <v>211.793</v>
-      </c>
-      <c r="D490" t="n">
-        <v>-104.177</v>
-      </c>
-      <c r="E490" t="n">
-        <v>5672.205</v>
-      </c>
-      <c r="F490" t="n">
-        <v>23.92</v>
-      </c>
-      <c r="G490" t="n">
-        <v>1003.631</v>
-      </c>
-      <c r="H490" t="n">
-        <v>-1.052</v>
-      </c>
-      <c r="I490" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="491" spans="1:9">
-      <c r="A491" t="n">
-        <v>489</v>
-      </c>
-      <c r="B491" t="n">
-        <v>5697.545</v>
-      </c>
-      <c r="C491" t="n">
-        <v>211.688</v>
-      </c>
-      <c r="D491" t="n">
-        <v>-105.672</v>
-      </c>
-      <c r="E491" t="n">
-        <v>5695.857</v>
-      </c>
-      <c r="F491" t="n">
-        <v>23.918</v>
-      </c>
-      <c r="G491" t="n">
-        <v>1009.315</v>
-      </c>
-      <c r="H491" t="n">
-        <v>-1.062</v>
-      </c>
-      <c r="I491" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="492" spans="1:9">
-      <c r="A492" t="n">
-        <v>490</v>
-      </c>
-      <c r="B492" t="n">
-        <v>5721.634</v>
-      </c>
-      <c r="C492" t="n">
-        <v>211.58</v>
-      </c>
-      <c r="D492" t="n">
-        <v>-107.169</v>
-      </c>
-      <c r="E492" t="n">
-        <v>5719.517</v>
-      </c>
-      <c r="F492" t="n">
-        <v>23.916</v>
-      </c>
-      <c r="G492" t="n">
-        <v>1015.022</v>
-      </c>
-      <c r="H492" t="n">
-        <v>-1.073</v>
-      </c>
-      <c r="I492" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="493" spans="1:9">
-      <c r="A493" t="n">
-        <v>491</v>
-      </c>
-      <c r="B493" t="n">
-        <v>5745.723</v>
-      </c>
-      <c r="C493" t="n">
-        <v>211.472</v>
-      </c>
-      <c r="D493" t="n">
-        <v>-108.665</v>
-      </c>
-      <c r="E493" t="n">
-        <v>5743.5</v>
-      </c>
-      <c r="F493" t="n">
-        <v>23.915</v>
-      </c>
-      <c r="G493" t="n">
-        <v>1020.754</v>
-      </c>
-      <c r="H493" t="n">
-        <v>-1.083</v>
-      </c>
-      <c r="I493" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="494" spans="1:9">
-      <c r="A494" t="n">
-        <v>492</v>
-      </c>
-      <c r="B494" t="n">
-        <v>5769.812</v>
-      </c>
-      <c r="C494" t="n">
-        <v>211.362</v>
-      </c>
-      <c r="D494" t="n">
-        <v>-110.163</v>
-      </c>
-      <c r="E494" t="n">
-        <v>5768.131</v>
-      </c>
-      <c r="F494" t="n">
-        <v>23.913</v>
-      </c>
-      <c r="G494" t="n">
-        <v>1026.51</v>
-      </c>
-      <c r="H494" t="n">
-        <v>-1.093</v>
-      </c>
-      <c r="I494" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="495" spans="1:9">
-      <c r="A495" t="n">
-        <v>493</v>
-      </c>
-      <c r="B495" t="n">
-        <v>5793.901</v>
-      </c>
-      <c r="C495" t="n">
-        <v>211.25</v>
-      </c>
-      <c r="D495" t="n">
-        <v>-111.66</v>
-      </c>
-      <c r="E495" t="n">
-        <v>5793.641</v>
-      </c>
-      <c r="F495" t="n">
-        <v>24.155</v>
-      </c>
-      <c r="G495" t="n">
-        <v>1032.291</v>
-      </c>
-      <c r="H495" t="n">
-        <v>-1.103</v>
-      </c>
-      <c r="I495" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="496" spans="1:9">
-      <c r="A496" t="n">
-        <v>494</v>
-      </c>
-      <c r="B496" t="n">
-        <v>5817.989</v>
-      </c>
-      <c r="C496" t="n">
-        <v>211.137</v>
-      </c>
-      <c r="D496" t="n">
-        <v>-113.158</v>
-      </c>
-      <c r="E496" t="n">
-        <v>5817.989</v>
-      </c>
-      <c r="F496" t="n">
-        <v>25.055</v>
-      </c>
-      <c r="G496" t="n">
-        <v>1038.096</v>
-      </c>
-      <c r="H496" t="n">
-        <v>-1.112</v>
-      </c>
-      <c r="I496" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="497" spans="1:9">
-      <c r="A497" t="n">
-        <v>495</v>
-      </c>
-      <c r="B497" t="n">
-        <v>5844.697</v>
-      </c>
-      <c r="C497" t="n">
-        <v>211.022</v>
-      </c>
-      <c r="D497" t="n">
-        <v>-114.657</v>
-      </c>
-      <c r="E497" t="n">
-        <v>5844.697</v>
-      </c>
-      <c r="F497" t="n">
-        <v>27.215</v>
-      </c>
-      <c r="G497" t="n">
-        <v>1043.928</v>
-      </c>
-      <c r="H497" t="n">
-        <v>-1.121</v>
-      </c>
-      <c r="I497" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="498" spans="1:9">
-      <c r="A498" t="n">
-        <v>496</v>
-      </c>
-      <c r="B498" t="n">
-        <v>5875.638</v>
-      </c>
-      <c r="C498" t="n">
-        <v>210.906</v>
-      </c>
-      <c r="D498" t="n">
-        <v>-116.156</v>
-      </c>
-      <c r="E498" t="n">
-        <v>5875.638</v>
-      </c>
-      <c r="F498" t="n">
-        <v>29.348</v>
-      </c>
-      <c r="G498" t="n">
-        <v>1049.788</v>
-      </c>
-      <c r="H498" t="n">
-        <v>-1.13</v>
-      </c>
-      <c r="I498" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="499" spans="1:9">
-      <c r="A499" t="n">
-        <v>497</v>
-      </c>
-      <c r="B499" t="n">
-        <v>5907.663</v>
-      </c>
-      <c r="C499" t="n">
-        <v>210.788</v>
-      </c>
-      <c r="D499" t="n">
-        <v>-117.65</v>
-      </c>
-      <c r="E499" t="n">
-        <v>5906.151</v>
-      </c>
-      <c r="F499" t="n">
-        <v>30.897</v>
-      </c>
-      <c r="G499" t="n">
-        <v>1055.679</v>
-      </c>
-      <c r="H499" t="n">
-        <v>-1.138</v>
-      </c>
-      <c r="I499" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="500" spans="1:9">
-      <c r="A500" t="n">
-        <v>498</v>
-      </c>
-      <c r="B500" t="n">
-        <v>5939.267</v>
-      </c>
-      <c r="C500" t="n">
-        <v>210.669</v>
-      </c>
-      <c r="D500" t="n">
-        <v>-119.122</v>
-      </c>
-      <c r="E500" t="n">
-        <v>5936.986</v>
-      </c>
-      <c r="F500" t="n">
-        <v>31.259</v>
-      </c>
-      <c r="G500" t="n">
-        <v>1061.6</v>
-      </c>
-      <c r="H500" t="n">
-        <v>-1.145</v>
-      </c>
-      <c r="I500" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="501" spans="1:9">
-      <c r="A501" t="n">
-        <v>499</v>
-      </c>
-      <c r="B501" t="n">
-        <v>5971.717</v>
-      </c>
-      <c r="C501" t="n">
-        <v>210.548</v>
-      </c>
-      <c r="D501" t="n">
-        <v>-120.536</v>
-      </c>
-      <c r="E501" t="n">
-        <v>5968.747</v>
-      </c>
-      <c r="F501" t="n">
-        <v>31.526</v>
-      </c>
-      <c r="G501" t="n">
-        <v>1067.553</v>
-      </c>
-      <c r="H501" t="n">
-        <v>-1.15</v>
-      </c>
-      <c r="I501" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="502" spans="1:9">
-      <c r="A502" t="n">
-        <v>500</v>
-      </c>
-      <c r="B502" t="n">
-        <v>6003.08</v>
-      </c>
-      <c r="C502" t="n">
-        <v>210.426</v>
-      </c>
-      <c r="D502" t="n">
-        <v>-121.822</v>
-      </c>
-      <c r="E502" t="n">
-        <v>6001.265</v>
-      </c>
-      <c r="F502" t="n">
-        <v>31.907</v>
-      </c>
-      <c r="G502" t="n">
-        <v>1073.538</v>
-      </c>
-      <c r="H502" t="n">
-        <v>-1.154</v>
-      </c>
-      <c r="I502" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="503" spans="1:9">
-      <c r="A503" t="n">
-        <v>501</v>
-      </c>
-      <c r="B503" t="n">
-        <v>6034.433</v>
-      </c>
-      <c r="C503" t="n">
-        <v>210.303</v>
-      </c>
-      <c r="D503" t="n">
-        <v>-122.897</v>
-      </c>
-      <c r="E503" t="n">
-        <v>6034.195</v>
-      </c>
-      <c r="F503" t="n">
-        <v>32.358</v>
-      </c>
-      <c r="G503" t="n">
-        <v>1079.556</v>
-      </c>
-      <c r="H503" t="n">
-        <v>-1.154</v>
-      </c>
-      <c r="I503" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="504" spans="1:9">
-      <c r="A504" t="n">
-        <v>502</v>
-      </c>
-      <c r="B504" t="n">
-        <v>6068.291</v>
-      </c>
-      <c r="C504" t="n">
-        <v>210.178</v>
-      </c>
-      <c r="D504" t="n">
-        <v>-123.703</v>
-      </c>
-      <c r="E504" t="n">
-        <v>6067.247</v>
-      </c>
-      <c r="F504" t="n">
-        <v>32.826</v>
-      </c>
-      <c r="G504" t="n">
-        <v>1085.607</v>
-      </c>
-      <c r="H504" t="n">
-        <v>-1.154</v>
-      </c>
-      <c r="I504" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="505" spans="1:9">
-      <c r="A505" t="n">
-        <v>503</v>
-      </c>
-      <c r="B505" t="n">
-        <v>6101.616</v>
-      </c>
-      <c r="C505" t="n">
-        <v>210.053</v>
-      </c>
-      <c r="D505" t="n">
-        <v>-124.231</v>
-      </c>
-      <c r="E505" t="n">
-        <v>6100.375</v>
-      </c>
-      <c r="F505" t="n">
-        <v>33.153</v>
-      </c>
-      <c r="G505" t="n">
-        <v>1091.69</v>
-      </c>
-      <c r="H505" t="n">
-        <v>-1.154</v>
-      </c>
-      <c r="I505" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="506" spans="1:9">
-      <c r="A506" t="n">
-        <v>504</v>
-      </c>
-      <c r="B506" t="n">
-        <v>6134.899</v>
-      </c>
-      <c r="C506" t="n">
-        <v>209.928</v>
-      </c>
-      <c r="D506" t="n">
-        <v>-124.466</v>
-      </c>
-      <c r="E506" t="n">
-        <v>6133.714</v>
-      </c>
-      <c r="F506" t="n">
-        <v>33.377</v>
-      </c>
-      <c r="G506" t="n">
-        <v>1097.808</v>
-      </c>
-      <c r="H506" t="n">
-        <v>-1.15</v>
-      </c>
-      <c r="I506" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="507" spans="1:9">
-      <c r="A507" t="n">
-        <v>505</v>
-      </c>
-      <c r="B507" t="n">
-        <v>6169.343</v>
-      </c>
-      <c r="C507" t="n">
-        <v>209.803</v>
-      </c>
-      <c r="D507" t="n">
-        <v>-124.405</v>
-      </c>
-      <c r="E507" t="n">
-        <v>6167.396</v>
-      </c>
-      <c r="F507" t="n">
-        <v>33.497</v>
-      </c>
-      <c r="G507" t="n">
-        <v>1103.958</v>
-      </c>
-      <c r="H507" t="n">
-        <v>-1.143</v>
-      </c>
-      <c r="I507" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="508" spans="1:9">
-      <c r="A508" t="n">
-        <v>506</v>
-      </c>
-      <c r="B508" t="n">
-        <v>6203.03</v>
-      </c>
-      <c r="C508" t="n">
-        <v>209.678</v>
-      </c>
-      <c r="D508" t="n">
-        <v>-124.029</v>
-      </c>
-      <c r="E508" t="n">
-        <v>6201.445</v>
-      </c>
-      <c r="F508" t="n">
-        <v>33.657</v>
-      </c>
-      <c r="G508" t="n">
-        <v>1110.142</v>
-      </c>
-      <c r="H508" t="n">
-        <v>-1.132</v>
-      </c>
-      <c r="I508" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="509" spans="1:9">
-      <c r="A509" t="n">
-        <v>507</v>
-      </c>
-      <c r="B509" t="n">
-        <v>6237.023</v>
-      </c>
-      <c r="C509" t="n">
-        <v>209.554</v>
-      </c>
-      <c r="D509" t="n">
-        <v>-123.326</v>
-      </c>
-      <c r="E509" t="n">
-        <v>6235.842</v>
-      </c>
-      <c r="F509" t="n">
-        <v>33.906</v>
-      </c>
-      <c r="G509" t="n">
-        <v>1116.361</v>
-      </c>
-      <c r="H509" t="n">
-        <v>-1.119</v>
-      </c>
-      <c r="I509" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="510" spans="1:9">
-      <c r="A510" t="n">
-        <v>508</v>
-      </c>
-      <c r="B510" t="n">
-        <v>6270.538</v>
-      </c>
-      <c r="C510" t="n">
-        <v>209.431</v>
-      </c>
-      <c r="D510" t="n">
-        <v>-122.241</v>
-      </c>
-      <c r="E510" t="n">
-        <v>6270.538</v>
-      </c>
-      <c r="F510" t="n">
-        <v>34.284</v>
-      </c>
-      <c r="G510" t="n">
-        <v>1122.614</v>
-      </c>
-      <c r="H510" t="n">
-        <v>-1.102</v>
-      </c>
-      <c r="I510" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="511" spans="1:9">
-      <c r="A511" t="n">
-        <v>509</v>
-      </c>
-      <c r="B511" t="n">
-        <v>6305.984</v>
-      </c>
-      <c r="C511" t="n">
-        <v>209.31</v>
-      </c>
-      <c r="D511" t="n">
-        <v>-120.742</v>
-      </c>
-      <c r="E511" t="n">
-        <v>6305.561</v>
-      </c>
-      <c r="F511" t="n">
-        <v>34.725</v>
-      </c>
-      <c r="G511" t="n">
-        <v>1128.902</v>
-      </c>
-      <c r="H511" t="n">
-        <v>-1.082</v>
-      </c>
-      <c r="I511" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="512" spans="1:9">
-      <c r="A512" t="n">
-        <v>510</v>
-      </c>
-      <c r="B512" t="n">
-        <v>6342.398</v>
-      </c>
-      <c r="C512" t="n">
-        <v>209.19</v>
-      </c>
-      <c r="D512" t="n">
-        <v>-118.821</v>
-      </c>
-      <c r="E512" t="n">
-        <v>6340.823</v>
-      </c>
-      <c r="F512" t="n">
-        <v>35.183</v>
-      </c>
-      <c r="G512" t="n">
-        <v>1135.226</v>
-      </c>
-      <c r="H512" t="n">
-        <v>-1.058</v>
-      </c>
-      <c r="I512" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="513" spans="1:9">
-      <c r="A513" t="n">
-        <v>511</v>
-      </c>
-      <c r="B513" t="n">
-        <v>6377.247</v>
-      </c>
-      <c r="C513" t="n">
-        <v>209.073</v>
-      </c>
-      <c r="D513" t="n">
-        <v>-116.495</v>
-      </c>
-      <c r="E513" t="n">
-        <v>6376.349</v>
-      </c>
-      <c r="F513" t="n">
-        <v>35.576</v>
-      </c>
-      <c r="G513" t="n">
-        <v>1141.584</v>
-      </c>
-      <c r="H513" t="n">
-        <v>-1.031</v>
-      </c>
-      <c r="I513" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="514" spans="1:9">
-      <c r="A514" t="n">
-        <v>512</v>
-      </c>
-      <c r="B514" t="n">
-        <v>6413.014</v>
-      </c>
-      <c r="C514" t="n">
-        <v>208.959</v>
-      </c>
-      <c r="D514" t="n">
-        <v>-113.755</v>
-      </c>
-      <c r="E514" t="n">
-        <v>6412.109</v>
-      </c>
-      <c r="F514" t="n">
-        <v>35.884</v>
-      </c>
-      <c r="G514" t="n">
-        <v>1147.978</v>
-      </c>
-      <c r="H514" t="n">
-        <v>-1.002</v>
-      </c>
-      <c r="I514" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="515" spans="1:9">
-      <c r="A515" t="n">
-        <v>513</v>
-      </c>
-      <c r="B515" t="n">
-        <v>6449.697</v>
-      </c>
-      <c r="C515" t="n">
-        <v>208.847</v>
-      </c>
-      <c r="D515" t="n">
-        <v>-110.6</v>
-      </c>
-      <c r="E515" t="n">
-        <v>6448.139</v>
-      </c>
-      <c r="F515" t="n">
-        <v>36.067</v>
-      </c>
-      <c r="G515" t="n">
-        <v>1154.408</v>
-      </c>
-      <c r="H515" t="n">
-        <v>-0.969</v>
-      </c>
-      <c r="I515" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="516" spans="1:9">
-      <c r="A516" t="n">
-        <v>514</v>
-      </c>
-      <c r="B516" t="n">
-        <v>6486.06</v>
-      </c>
-      <c r="C516" t="n">
-        <v>208.74</v>
-      </c>
-      <c r="D516" t="n">
-        <v>-107.041</v>
-      </c>
-      <c r="E516" t="n">
-        <v>6484.503</v>
-      </c>
-      <c r="F516" t="n">
-        <v>36.19</v>
-      </c>
-      <c r="G516" t="n">
-        <v>1160.875</v>
-      </c>
-      <c r="H516" t="n">
-        <v>-0.9350000000000001</v>
-      </c>
-      <c r="I516" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="517" spans="1:9">
-      <c r="A517" t="n">
-        <v>515</v>
-      </c>
-      <c r="B517" t="n">
-        <v>6522.226</v>
-      </c>
-      <c r="C517" t="n">
-        <v>208.636</v>
-      </c>
-      <c r="D517" t="n">
-        <v>-103.118</v>
-      </c>
-      <c r="E517" t="n">
-        <v>6521.189</v>
-      </c>
-      <c r="F517" t="n">
-        <v>36.288</v>
-      </c>
-      <c r="G517" t="n">
-        <v>1167.378</v>
-      </c>
-      <c r="H517" t="n">
-        <v>-0.899</v>
-      </c>
-      <c r="I517" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="518" spans="1:9">
-      <c r="A518" t="n">
-        <v>516</v>
-      </c>
-      <c r="B518" t="n">
-        <v>6558.535</v>
-      </c>
-      <c r="C518" t="n">
-        <v>208.537</v>
-      </c>
-      <c r="D518" t="n">
-        <v>-98.919</v>
-      </c>
-      <c r="E518" t="n">
-        <v>6558.222</v>
-      </c>
-      <c r="F518" t="n">
-        <v>36.547</v>
-      </c>
-      <c r="G518" t="n">
-        <v>1173.917</v>
-      </c>
-      <c r="H518" t="n">
-        <v>-0.862</v>
-      </c>
-      <c r="I518" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="519" spans="1:9">
-      <c r="A519" t="n">
-        <v>517</v>
-      </c>
-      <c r="B519" t="n">
-        <v>6595.16</v>
-      </c>
-      <c r="C519" t="n">
-        <v>208.442</v>
-      </c>
-      <c r="D519" t="n">
-        <v>-94.57299999999999</v>
-      </c>
-      <c r="E519" t="n">
-        <v>6595.16</v>
-      </c>
-      <c r="F519" t="n">
-        <v>36.957</v>
-      </c>
-      <c r="G519" t="n">
-        <v>1180.494</v>
-      </c>
-      <c r="H519" t="n">
-        <v>-0.824</v>
-      </c>
-      <c r="I519" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="520" spans="1:9">
-      <c r="A520" t="n">
-        <v>518</v>
-      </c>
-      <c r="B520" t="n">
-        <v>6633.173</v>
-      </c>
-      <c r="C520" t="n">
-        <v>208.352</v>
-      </c>
-      <c r="D520" t="n">
-        <v>-90.233</v>
-      </c>
-      <c r="E520" t="n">
-        <v>6633.173</v>
-      </c>
-      <c r="F520" t="n">
-        <v>37.579</v>
-      </c>
-      <c r="G520" t="n">
-        <v>1187.108</v>
-      </c>
-      <c r="H520" t="n">
-        <v>-0.787</v>
-      </c>
-      <c r="I520" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="521" spans="1:9">
-      <c r="A521" t="n">
-        <v>519</v>
-      </c>
-      <c r="B521" t="n">
-        <v>6671.464</v>
-      </c>
-      <c r="C521" t="n">
-        <v>208.267</v>
-      </c>
-      <c r="D521" t="n">
-        <v>-86.048</v>
-      </c>
-      <c r="E521" t="n">
-        <v>6671.464</v>
-      </c>
-      <c r="F521" t="n">
-        <v>38.186</v>
-      </c>
-      <c r="G521" t="n">
-        <v>1193.761</v>
-      </c>
-      <c r="H521" t="n">
-        <v>-0.75</v>
-      </c>
-      <c r="I521" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="522" spans="1:9">
-      <c r="A522" t="n">
-        <v>520</v>
-      </c>
-      <c r="B522" t="n">
-        <v>6711.186</v>
-      </c>
-      <c r="C522" t="n">
-        <v>208.185</v>
-      </c>
-      <c r="D522" t="n">
-        <v>-82.14</v>
-      </c>
-      <c r="E522" t="n">
-        <v>6710.309</v>
-      </c>
-      <c r="F522" t="n">
-        <v>38.763</v>
-      </c>
-      <c r="G522" t="n">
-        <v>1200.451</v>
-      </c>
-      <c r="H522" t="n">
-        <v>-0.716</v>
-      </c>
-      <c r="I522" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="523" spans="1:9">
-      <c r="A523" t="n">
-        <v>521</v>
-      </c>
-      <c r="B523" t="n">
-        <v>6750.715</v>
-      </c>
-      <c r="C523" t="n">
-        <v>208.107</v>
-      </c>
-      <c r="D523" t="n">
-        <v>-78.584</v>
-      </c>
-      <c r="E523" t="n">
-        <v>6749.486</v>
-      </c>
-      <c r="F523" t="n">
-        <v>39.188</v>
-      </c>
-      <c r="G523" t="n">
-        <v>1207.181</v>
-      </c>
-      <c r="H523" t="n">
-        <v>-0.6830000000000001</v>
-      </c>
-      <c r="I523" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="524" spans="1:9">
-      <c r="A524" t="n">
-        <v>522</v>
-      </c>
-      <c r="B524" t="n">
-        <v>6789.57</v>
-      </c>
-      <c r="C524" t="n">
-        <v>208.033</v>
-      </c>
-      <c r="D524" t="n">
-        <v>-75.411</v>
-      </c>
-      <c r="E524" t="n">
-        <v>6789.18</v>
-      </c>
-      <c r="F524" t="n">
-        <v>39.493</v>
-      </c>
-      <c r="G524" t="n">
-        <v>1213.951</v>
-      </c>
-      <c r="H524" t="n">
-        <v>-0.653</v>
-      </c>
-      <c r="I524" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="525" spans="1:9">
-      <c r="A525" t="n">
-        <v>523</v>
-      </c>
-      <c r="B525" t="n">
-        <v>6829.259</v>
-      </c>
-      <c r="C525" t="n">
-        <v>207.961</v>
-      </c>
-      <c r="D525" t="n">
-        <v>-72.63</v>
-      </c>
-      <c r="E525" t="n">
-        <v>6829.259</v>
-      </c>
-      <c r="F525" t="n">
-        <v>39.72</v>
-      </c>
-      <c r="G525" t="n">
-        <v>1220.76</v>
-      </c>
-      <c r="H525" t="n">
-        <v>-0.626</v>
-      </c>
-      <c r="I525" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="526" spans="1:9">
-      <c r="A526" t="n">
-        <v>524</v>
-      </c>
-      <c r="B526" t="n">
-        <v>6869.225</v>
-      </c>
-      <c r="C526" t="n">
-        <v>207.891</v>
-      </c>
-      <c r="D526" t="n">
-        <v>-70.241</v>
-      </c>
-      <c r="E526" t="n">
-        <v>6869.225</v>
-      </c>
-      <c r="F526" t="n">
-        <v>39.924</v>
-      </c>
-      <c r="G526" t="n">
-        <v>1227.609</v>
-      </c>
-      <c r="H526" t="n">
-        <v>-0.602</v>
-      </c>
-      <c r="I526" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="527" spans="1:9">
-      <c r="A527" t="n">
-        <v>525</v>
-      </c>
-      <c r="B527" t="n">
-        <v>6910.294</v>
-      </c>
-      <c r="C527" t="n">
-        <v>207.824</v>
-      </c>
-      <c r="D527" t="n">
-        <v>-68.244</v>
-      </c>
-      <c r="E527" t="n">
-        <v>6910.286</v>
-      </c>
-      <c r="F527" t="n">
-        <v>40.195</v>
-      </c>
-      <c r="G527" t="n">
-        <v>1234.499</v>
-      </c>
-      <c r="H527" t="n">
-        <v>-0.582</v>
-      </c>
-      <c r="I527" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="528" spans="1:9">
-      <c r="A528" t="n">
-        <v>526</v>
-      </c>
-      <c r="B528" t="n">
-        <v>6950.681</v>
-      </c>
-      <c r="C528" t="n">
-        <v>207.758</v>
-      </c>
-      <c r="D528" t="n">
-        <v>-66.66800000000001</v>
-      </c>
-      <c r="E528" t="n">
-        <v>6950.681</v>
-      </c>
-      <c r="F528" t="n">
-        <v>40.457</v>
-      </c>
-      <c r="G528" t="n">
-        <v>1241.429</v>
-      </c>
-      <c r="H528" t="n">
-        <v>-0.5649999999999999</v>
-      </c>
-      <c r="I528" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="529" spans="1:9">
-      <c r="A529" t="n">
-        <v>527</v>
-      </c>
-      <c r="B529" t="n">
-        <v>6993.409</v>
-      </c>
-      <c r="C529" t="n">
-        <v>207.693</v>
-      </c>
-      <c r="D529" t="n">
-        <v>-65.515</v>
-      </c>
-      <c r="E529" t="n">
-        <v>6992.042</v>
-      </c>
-      <c r="F529" t="n">
-        <v>40.713</v>
-      </c>
-      <c r="G529" t="n">
-        <v>1248.401</v>
-      </c>
-      <c r="H529" t="n">
-        <v>-0.551</v>
-      </c>
-      <c r="I529" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="530" spans="1:9">
-      <c r="A530" t="n">
-        <v>528</v>
-      </c>
-      <c r="B530" t="n">
-        <v>7034.419</v>
-      </c>
-      <c r="C530" t="n">
-        <v>207.629</v>
-      </c>
-      <c r="D530" t="n">
-        <v>-64.761</v>
-      </c>
-      <c r="E530" t="n">
-        <v>7033.171</v>
-      </c>
-      <c r="F530" t="n">
-        <v>40.86</v>
-      </c>
-      <c r="G530" t="n">
-        <v>1255.413</v>
-      </c>
-      <c r="H530" t="n">
-        <v>-0.541</v>
-      </c>
-      <c r="I530" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="531" spans="1:9">
-      <c r="A531" t="n">
-        <v>529</v>
-      </c>
-      <c r="B531" t="n">
-        <v>7074.056</v>
-      </c>
-      <c r="C531" t="n">
-        <v>207.565</v>
-      </c>
-      <c r="D531" t="n">
-        <v>-64.352</v>
-      </c>
-      <c r="E531" t="n">
-        <v>7074.056</v>
-      </c>
-      <c r="F531" t="n">
-        <v>40.936</v>
-      </c>
-      <c r="G531" t="n">
-        <v>1262.467</v>
-      </c>
-      <c r="H531" t="n">
-        <v>-0.533</v>
-      </c>
-      <c r="I531" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="532" spans="1:9">
-      <c r="A532" t="n">
-        <v>530</v>
-      </c>
-      <c r="B532" t="n">
-        <v>7116.246</v>
-      </c>
-      <c r="C532" t="n">
-        <v>207.502</v>
-      </c>
-      <c r="D532" t="n">
-        <v>-64.261</v>
-      </c>
-      <c r="E532" t="n">
-        <v>7116.246</v>
-      </c>
-      <c r="F532" t="n">
-        <v>40.949</v>
-      </c>
-      <c r="G532" t="n">
-        <v>1269.562</v>
-      </c>
-      <c r="H532" t="n">
-        <v>-0.528</v>
-      </c>
-      <c r="I532" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="533" spans="1:9">
-      <c r="A533" t="n">
-        <v>531</v>
-      </c>
-      <c r="B533" t="n">
-        <v>7157.243</v>
-      </c>
-      <c r="C533" t="n">
-        <v>207.438</v>
-      </c>
-      <c r="D533" t="n">
-        <v>-64.44499999999999</v>
-      </c>
-      <c r="E533" t="n">
-        <v>7157.243</v>
-      </c>
-      <c r="F533" t="n">
-        <v>40.956</v>
-      </c>
-      <c r="G533" t="n">
-        <v>1276.699</v>
-      </c>
-      <c r="H533" t="n">
-        <v>-0.528</v>
-      </c>
-      <c r="I533" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="534" spans="1:9">
-      <c r="A534" t="n">
-        <v>532</v>
-      </c>
-      <c r="B534" t="n">
-        <v>7198.308</v>
-      </c>
-      <c r="C534" t="n">
-        <v>207.374</v>
-      </c>
-      <c r="D534" t="n">
-        <v>-64.879</v>
-      </c>
-      <c r="E534" t="n">
-        <v>7198.308</v>
-      </c>
-      <c r="F534" t="n">
-        <v>40.968</v>
-      </c>
-      <c r="G534" t="n">
-        <v>1283.877</v>
-      </c>
-      <c r="H534" t="n">
-        <v>-0.528</v>
-      </c>
-      <c r="I534" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="535" spans="1:9">
-      <c r="A535" t="n">
-        <v>533</v>
-      </c>
-      <c r="B535" t="n">
-        <v>7240.034</v>
-      </c>
-      <c r="C535" t="n">
-        <v>207.309</v>
-      </c>
-      <c r="D535" t="n">
-        <v>-65.547</v>
-      </c>
-      <c r="E535" t="n">
-        <v>7240.034</v>
-      </c>
-      <c r="F535" t="n">
-        <v>41.003</v>
-      </c>
-      <c r="G535" t="n">
-        <v>1291.096</v>
-      </c>
-      <c r="H535" t="n">
-        <v>-0.528</v>
-      </c>
-      <c r="I535" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <drawing r:id="rId1"/>

</xml_diff>